<commit_message>
Upload functionality and displaying
</commit_message>
<xml_diff>
--- a/uploads/excel/Quickbooks.xlsx
+++ b/uploads/excel/Quickbooks.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-Asus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\For Henne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4815901-536D-49E6-A61C-F7BFD736E0D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QuickBooks Desktop Export Tips" sheetId="2" r:id="rId1"/>
@@ -71,16 +70,10 @@
     <definedName name="QBROWHEADERS" localSheetId="1">1</definedName>
     <definedName name="QBSTARTDATE" localSheetId="1">20190801</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -437,9 +430,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00;\-#,##0.00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -523,11 +517,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="39" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="39" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="39" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -545,7 +539,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -577,13 +571,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -901,7 +889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H40"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="84" zoomScaleNormal="84" workbookViewId="0"/>
@@ -1785,11 +1773,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1350" ySplit="615" topLeftCell="B1" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>